<commit_message>
feat: add construction impacts to impact calculator
</commit_message>
<xml_diff>
--- a/references/background_data/a5_wastage.xlsx
+++ b/references/background_data/a5_wastage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchaf\Documents\GitHub_CLF\pod_lca_data_analysis\references\background_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02552FE8-F2EF-4240-9C48-5D1839489D8C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6002BBEA-DD48-48D2-A84C-75B57BAB75F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
-    <t>Wastage</t>
-  </si>
-  <si>
     <t>Building Material_name</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t>unsure</t>
+  </si>
+  <si>
+    <t>wastage</t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -548,15 +548,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>0.05</v>
@@ -564,7 +564,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>0.03</v>
@@ -572,7 +572,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>0.03</v>
@@ -580,7 +580,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>0.05</v>
@@ -588,7 +588,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>0.1</v>
@@ -596,7 +596,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>0.05</v>
@@ -604,7 +604,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>0.05</v>
@@ -612,7 +612,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>0.1</v>
@@ -620,7 +620,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>0.1</v>
@@ -628,7 +628,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>0.1</v>
@@ -636,7 +636,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>0.05</v>
@@ -644,7 +644,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>0.03</v>
@@ -652,7 +652,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>0.1</v>
@@ -660,7 +660,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>0.03</v>
@@ -668,7 +668,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>0.15</v>
@@ -676,7 +676,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>0.1</v>
@@ -684,7 +684,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>0.01</v>
@@ -692,18 +692,18 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>0.05</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>0.15</v>
@@ -711,7 +711,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21">
         <v>0.1</v>
@@ -719,7 +719,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>0.1</v>
@@ -727,7 +727,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>0.1</v>
@@ -735,7 +735,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24">
         <v>0.15</v>
@@ -743,7 +743,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25">
         <v>0.1</v>
@@ -751,7 +751,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26">
         <v>0.15</v>
@@ -759,7 +759,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27">
         <v>0.05</v>
@@ -767,7 +767,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28">
         <v>0.1</v>
@@ -775,18 +775,18 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29">
         <v>0.05</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30">
         <v>0.15</v>
@@ -794,7 +794,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31">
         <v>0.15</v>
@@ -802,7 +802,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32">
         <v>0.15</v>
@@ -810,7 +810,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33">
         <v>0.1</v>
@@ -818,7 +818,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34">
         <v>0.1</v>
@@ -826,7 +826,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35">
         <v>0.05</v>
@@ -834,7 +834,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36">
         <v>0.1</v>
@@ -842,7 +842,7 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37">
         <v>0.1</v>
@@ -850,7 +850,7 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B38">
         <v>0.05</v>
@@ -858,7 +858,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39">
         <v>0.1</v>
@@ -866,18 +866,18 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40">
         <v>0.1</v>
       </c>
       <c r="C40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41">
         <v>0.1</v>
@@ -885,7 +885,7 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42">
         <v>0.1</v>
@@ -893,7 +893,7 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43">
         <v>0.1</v>
@@ -901,7 +901,7 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44">
         <v>0.1</v>
@@ -909,7 +909,7 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45">
         <v>0.05</v>
@@ -917,7 +917,7 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46">
         <v>0.1</v>
@@ -925,7 +925,7 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47">
         <v>0.01</v>
@@ -933,7 +933,7 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48">
         <v>0.01</v>
@@ -941,7 +941,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49">
         <v>0.15</v>
@@ -949,7 +949,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B50">
         <v>0.15</v>

</xml_diff>

<commit_message>
fix: all bom and wastage factor fixes for compatibility
</commit_message>
<xml_diff>
--- a/references/background_data/a5_wastage.xlsx
+++ b/references/background_data/a5_wastage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchaf\Documents\GitHub_CLF\pod_lca_data_analysis\references\background_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376CE672-EBF9-441B-BE84-CC622AA0F5F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC0B5EF-BC60-4E43-9D4F-3266E9D6645E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,9 +30,6 @@
     <t>Building Material_name</t>
   </si>
   <si>
-    <t>Normalweight Concrete, 4000 psi</t>
-  </si>
-  <si>
     <t>Steel, reinforcing rod</t>
   </si>
   <si>
@@ -48,45 +45,24 @@
     <t>Steel, hot rolled structural steel</t>
   </si>
   <si>
-    <t>Normalweight Concrete, 6000 psi</t>
-  </si>
-  <si>
-    <t>Normalweight Concrete, 5000 psi</t>
-  </si>
-  <si>
     <t>CLT (Cross laminated timber)</t>
   </si>
   <si>
     <t>Glue laminated timber (Glulam)</t>
   </si>
   <si>
-    <t>Steel Curtain Wall System</t>
-  </si>
-  <si>
     <t>Fluoropolymer coating, metal stock</t>
   </si>
   <si>
-    <t>5" mineral wool insulation</t>
-  </si>
-  <si>
     <t>Acrylic latex paint</t>
   </si>
   <si>
-    <t>Aluminum Curtain Wall System</t>
-  </si>
-  <si>
     <t>Brick</t>
   </si>
   <si>
-    <t>Type N Mortar</t>
-  </si>
-  <si>
     <t>Galvanized steel shelf angle with knife plate</t>
   </si>
   <si>
-    <t>4" mineral wool insulation</t>
-  </si>
-  <si>
     <t>AVB membrane</t>
   </si>
   <si>
@@ -108,79 +84,103 @@
     <t>Stainless steel fastener</t>
   </si>
   <si>
-    <t>3/8" Synthetic Stucco</t>
-  </si>
-  <si>
     <t>2.5" XPS insulation</t>
   </si>
   <si>
-    <t>Glass Fiber Reinforced Concrete (GFRC) Panel</t>
+    <t>3/4" Brick</t>
+  </si>
+  <si>
+    <t>Water based stain</t>
+  </si>
+  <si>
+    <t>Aluminum extrusion</t>
+  </si>
+  <si>
+    <t>Double pane IGU</t>
+  </si>
+  <si>
+    <t>Triple pane IGU</t>
+  </si>
+  <si>
+    <t>EPDM membrane</t>
+  </si>
+  <si>
+    <t>Polyisocyanurate board</t>
+  </si>
+  <si>
+    <t>unsure</t>
+  </si>
+  <si>
+    <t>wastage</t>
+  </si>
+  <si>
+    <t>6" galvanized steel stud framing</t>
+  </si>
+  <si>
+    <t>Gypsum wall board</t>
+  </si>
+  <si>
+    <t>Normalweight concrete, 4000 psi</t>
+  </si>
+  <si>
+    <t>Normalweight concrete, 6000 psi</t>
+  </si>
+  <si>
+    <t>Normalweight concrete, 5000 psi</t>
+  </si>
+  <si>
+    <t>Steel curtain wall system</t>
+  </si>
+  <si>
+    <t>Aluminum curtain wall system</t>
+  </si>
+  <si>
+    <t>Type N mortar</t>
+  </si>
+  <si>
+    <t>4" Mineral wool insulation</t>
+  </si>
+  <si>
+    <t>4.5" Mineral wool insulation</t>
+  </si>
+  <si>
+    <t>Glass fiber reinforced concrete (GFRC) Panel</t>
+  </si>
+  <si>
+    <t>3/8" Synthetic stucco</t>
+  </si>
+  <si>
+    <t>Galvanized steel backer tray</t>
+  </si>
+  <si>
+    <t>Steel, sheet</t>
+  </si>
+  <si>
+    <t>Thermal break</t>
+  </si>
+  <si>
+    <t>3.5" Mineral wool insulation</t>
+  </si>
+  <si>
+    <t>6" x 1' Tulipwood/Poplar lumber</t>
+  </si>
+  <si>
+    <t>Formed steel sheet</t>
+  </si>
+  <si>
+    <t>Enamel paint</t>
+  </si>
+  <si>
+    <t>Stainless steel fasteners</t>
+  </si>
+  <si>
+    <t>Galvanized steel support</t>
+  </si>
+  <si>
+    <t>5" Mineral wool insulation</t>
   </si>
   <si>
     <t>Galvanized steel support system</t>
-  </si>
-  <si>
-    <t>4.5" Mineral Wool insulation</t>
-  </si>
-  <si>
-    <t>3/4" Brick</t>
-  </si>
-  <si>
-    <t>Galvanized Steel Backer Tray</t>
-  </si>
-  <si>
-    <t>Steel, Sheet</t>
-  </si>
-  <si>
-    <t>Thermal Break</t>
-  </si>
-  <si>
-    <t>3.5" Mineral Wool insulation</t>
-  </si>
-  <si>
-    <t>6" x 1' Tulipwood/Poplar Lumber</t>
-  </si>
-  <si>
-    <t>Water based stain</t>
-  </si>
-  <si>
-    <t>Aluminum extrusion</t>
-  </si>
-  <si>
-    <t>Formed Steel Sheet</t>
-  </si>
-  <si>
-    <t>Enamel Paint</t>
-  </si>
-  <si>
-    <t>Stainless Steel Fasteners</t>
-  </si>
-  <si>
-    <t>Galvanized Steel Support</t>
-  </si>
-  <si>
-    <t>Double pane IGU</t>
-  </si>
-  <si>
-    <t>Triple pane IGU</t>
-  </si>
-  <si>
-    <t>EPDM membrane</t>
-  </si>
-  <si>
-    <t>Polyisocyanurate board</t>
-  </si>
-  <si>
-    <t>unsure</t>
-  </si>
-  <si>
-    <t>wastage</t>
-  </si>
-  <si>
-    <t>6" galvanized steel stud framing</t>
-  </si>
-  <si>
-    <t>Gypsum wall board</t>
   </si>
 </sst>
 </file>
@@ -537,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -551,12 +551,12 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="B2">
         <v>0.05</v>
@@ -564,7 +564,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>0.03</v>
@@ -572,7 +572,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>0.03</v>
@@ -580,7 +580,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>0.05</v>
@@ -588,7 +588,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>0.1</v>
@@ -596,7 +596,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>0.05</v>
@@ -604,7 +604,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B8">
         <v>0.05</v>
@@ -612,7 +612,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="4" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B9">
         <v>0.1</v>
@@ -620,7 +620,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10">
         <v>0.1</v>
@@ -628,7 +628,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B11">
         <v>0.1</v>
@@ -636,7 +636,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="B12">
         <v>0.05</v>
@@ -644,7 +644,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13">
         <v>0.03</v>
@@ -652,7 +652,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="B14">
         <v>0.1</v>
@@ -660,7 +660,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="B15">
         <v>0.03</v>
@@ -668,7 +668,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="B16">
         <v>0.15</v>
@@ -676,7 +676,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B17">
         <v>0.1</v>
@@ -684,7 +684,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B18">
         <v>0.01</v>
@@ -692,18 +692,18 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B19">
         <v>0.05</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="B20">
         <v>0.15</v>
@@ -711,7 +711,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B21">
         <v>0.1</v>
@@ -719,7 +719,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="B22">
         <v>0.1</v>
@@ -727,7 +727,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B23">
         <v>0.1</v>
@@ -735,7 +735,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B24">
         <v>0.15</v>
@@ -743,7 +743,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B25">
         <v>0.1</v>
@@ -751,7 +751,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B26">
         <v>0.15</v>
@@ -759,7 +759,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B27">
         <v>0.05</v>
@@ -767,7 +767,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B28">
         <v>0.1</v>
@@ -775,18 +775,18 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B29">
         <v>0.05</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="2" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B30">
         <v>0.15</v>
@@ -794,7 +794,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B31">
         <v>0.15</v>
@@ -802,7 +802,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B32">
         <v>0.15</v>
@@ -810,7 +810,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="B33">
         <v>0.1</v>
@@ -818,7 +818,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B34">
         <v>0.1</v>
@@ -826,7 +826,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B35">
         <v>0.05</v>
@@ -834,7 +834,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B36">
         <v>0.1</v>
@@ -842,7 +842,7 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="2" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B37">
         <v>0.1</v>
@@ -850,7 +850,7 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="2" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B38">
         <v>0.05</v>
@@ -858,7 +858,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="2" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B39">
         <v>0.1</v>
@@ -866,18 +866,18 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="2" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B40">
         <v>0.1</v>
       </c>
       <c r="C40" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="2" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="B41">
         <v>0.1</v>
@@ -885,7 +885,7 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="2" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B42">
         <v>0.1</v>
@@ -893,7 +893,7 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B43">
         <v>0.1</v>
@@ -901,7 +901,7 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B44">
         <v>0.1</v>
@@ -909,7 +909,7 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="2" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B45">
         <v>0.05</v>
@@ -917,7 +917,7 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="2" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B46">
         <v>0.1</v>
@@ -925,7 +925,7 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="2" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="B47">
         <v>0.01</v>
@@ -933,7 +933,7 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="2" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="B48">
         <v>0.01</v>
@@ -941,7 +941,7 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="2" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="B49">
         <v>0.15</v>
@@ -949,7 +949,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="2" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="B50">
         <v>0.15</v>

</xml_diff>

<commit_message>
feat: update wastage background dataset
</commit_message>
<xml_diff>
--- a/references/background_data/a5_wastage.xlsx
+++ b/references/background_data/a5_wastage.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchaf\Documents\GitHub_CLF\pod_lca_data_analysis\references\background_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC0B5EF-BC60-4E43-9D4F-3266E9D6645E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCF6C13-B72B-4635-9CEC-97CD385C55A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Building Material_name</t>
   </si>
@@ -108,9 +108,6 @@
     <t>Polyisocyanurate board</t>
   </si>
   <si>
-    <t>unsure</t>
-  </si>
-  <si>
     <t>wastage</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
   </si>
   <si>
     <t>Galvanized steel support system</t>
+  </si>
+  <si>
+    <t>enhanced wastage</t>
   </si>
 </sst>
 </file>
@@ -537,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -546,132 +546,180 @@
     <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8">
+        <v>0.05</v>
+      </c>
+      <c r="C8">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B8">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="B9">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B10">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B11">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B13">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16">
         <v>0.15</v>
+      </c>
+      <c r="C16">
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -681,13 +729,19 @@
       <c r="B17">
         <v>0.1</v>
       </c>
+      <c r="C17">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18">
         <v>0.01</v>
+      </c>
+      <c r="C18">
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -697,16 +751,19 @@
       <c r="B19">
         <v>0.05</v>
       </c>
-      <c r="C19" t="s">
-        <v>27</v>
+      <c r="C19">
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20">
         <v>0.15</v>
+      </c>
+      <c r="C20">
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -716,13 +773,19 @@
       <c r="B21">
         <v>0.1</v>
       </c>
+      <c r="C21">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22">
         <v>0.1</v>
+      </c>
+      <c r="C22">
+        <v>0.05</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -732,6 +795,9 @@
       <c r="B23">
         <v>0.1</v>
       </c>
+      <c r="C23">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
@@ -740,6 +806,9 @@
       <c r="B24">
         <v>0.15</v>
       </c>
+      <c r="C24">
+        <v>7.4999999999999997E-2</v>
+      </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
@@ -748,6 +817,9 @@
       <c r="B25">
         <v>0.1</v>
       </c>
+      <c r="C25">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="2" t="s">
@@ -756,6 +828,9 @@
       <c r="B26">
         <v>0.15</v>
       </c>
+      <c r="C26">
+        <v>7.4999999999999997E-2</v>
+      </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
@@ -764,6 +839,9 @@
       <c r="B27">
         <v>0.05</v>
       </c>
+      <c r="C27">
+        <v>2.5000000000000001E-2</v>
+      </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="2" t="s">
@@ -772,6 +850,9 @@
       <c r="B28">
         <v>0.1</v>
       </c>
+      <c r="C28">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
@@ -780,16 +861,19 @@
       <c r="B29">
         <v>0.05</v>
       </c>
-      <c r="C29" t="s">
-        <v>27</v>
+      <c r="C29">
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B30">
         <v>0.15</v>
+      </c>
+      <c r="C30">
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -799,29 +883,41 @@
       <c r="B31">
         <v>0.15</v>
       </c>
+      <c r="C31">
+        <v>7.4999999999999997E-2</v>
+      </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B32">
         <v>0.15</v>
       </c>
+      <c r="C32">
+        <v>7.4999999999999997E-2</v>
+      </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B33">
         <v>0.1</v>
+      </c>
+      <c r="C33">
+        <v>0.05</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B34">
         <v>0.1</v>
+      </c>
+      <c r="C34">
+        <v>0.05</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -831,48 +927,63 @@
       <c r="B35">
         <v>0.05</v>
       </c>
+      <c r="C35">
+        <v>2.5000000000000001E-2</v>
+      </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B36">
         <v>0.1</v>
+      </c>
+      <c r="C36">
+        <v>0.05</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B37">
         <v>0.1</v>
+      </c>
+      <c r="C37">
+        <v>0.05</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38">
         <v>0.05</v>
+      </c>
+      <c r="C38">
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B39">
         <v>0.1</v>
+      </c>
+      <c r="C39">
+        <v>0.05</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B40">
         <v>0.1</v>
       </c>
-      <c r="C40" t="s">
-        <v>27</v>
+      <c r="C40">
+        <v>0.05</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -882,6 +993,9 @@
       <c r="B41">
         <v>0.1</v>
       </c>
+      <c r="C41">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="2" t="s">
@@ -890,37 +1004,52 @@
       <c r="B42">
         <v>0.1</v>
       </c>
+      <c r="C42">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B43">
         <v>0.1</v>
+      </c>
+      <c r="C43">
+        <v>0.05</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B44">
         <v>0.1</v>
+      </c>
+      <c r="C44">
+        <v>0.05</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B45">
         <v>0.05</v>
+      </c>
+      <c r="C45">
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B46">
         <v>0.1</v>
+      </c>
+      <c r="C46">
+        <v>0.05</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -930,6 +1059,9 @@
       <c r="B47">
         <v>0.01</v>
       </c>
+      <c r="C47">
+        <v>5.0000000000000001E-3</v>
+      </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="2" t="s">
@@ -938,21 +1070,30 @@
       <c r="B48">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="C48">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
       <c r="A49" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B49">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
+      <c r="C49">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
       <c r="A50" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B50">
         <v>0.15</v>
+      </c>
+      <c r="C50">
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add prebuilt construction scenario
</commit_message>
<xml_diff>
--- a/references/background_data/a5_wastage.xlsx
+++ b/references/background_data/a5_wastage.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchaf\Documents\GitHub_CLF\pod_lca_data_analysis\references\background_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCF6C13-B72B-4635-9CEC-97CD385C55A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45088E9B-549F-449C-BAD9-CB3AAF947A36}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -538,7 +541,7 @@
   <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -576,7 +579,7 @@
         <v>0.03</v>
       </c>
       <c r="C3">
-        <v>0.05</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -587,7 +590,7 @@
         <v>0.03</v>
       </c>
       <c r="C4">
-        <v>0.05</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -598,7 +601,7 @@
         <v>0.05</v>
       </c>
       <c r="C5">
-        <v>1.4999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -609,7 +612,7 @@
         <v>0.1</v>
       </c>
       <c r="C6">
-        <v>1.4999999999999999E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -642,7 +645,7 @@
         <v>0.1</v>
       </c>
       <c r="C9">
-        <v>2.5000000000000001E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1097,6 +1100,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C1" xr:uid="{94B8B006-F0BE-45AC-AC61-F15B7818C7C2}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: created 180 new template models
</commit_message>
<xml_diff>
--- a/references/background_data/a5_wastage.xlsx
+++ b/references/background_data/a5_wastage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchaf\Documents\GitHub_CLF\pod_lca_data_analysis\references\background_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC386904-E9AB-4CFF-88CC-B710F627988D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9CB55F-DC0A-41B9-A64C-91D966E5C8CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,178 +42,178 @@
     <t>Lightweight concrete, 5000 psi</t>
   </si>
   <si>
+    <t>Steel, hot rolled structural steel</t>
+  </si>
+  <si>
+    <t>CLT (Cross laminated timber)</t>
+  </si>
+  <si>
+    <t>Glue laminated timber (Glulam)</t>
+  </si>
+  <si>
+    <t>Fluoropolymer coating, metal stock</t>
+  </si>
+  <si>
+    <t>Acrylic latex paint</t>
+  </si>
+  <si>
+    <t>Brick</t>
+  </si>
+  <si>
+    <t>Galvanized steel shelf angle with knife plate</t>
+  </si>
+  <si>
+    <t>AVB membrane</t>
+  </si>
+  <si>
+    <t>Sheathing</t>
+  </si>
+  <si>
+    <t>4" granite veneer</t>
+  </si>
+  <si>
+    <t>Type S mortar</t>
+  </si>
+  <si>
+    <t>Insulated 24 ga. steel sandwich panel with polyurethane foam</t>
+  </si>
+  <si>
+    <t>Fluoropolymer coating</t>
+  </si>
+  <si>
+    <t>Stainless steel fastener</t>
+  </si>
+  <si>
+    <t>2.5" XPS insulation</t>
+  </si>
+  <si>
+    <t>3/4" Brick</t>
+  </si>
+  <si>
+    <t>Water based stain</t>
+  </si>
+  <si>
+    <t>Aluminum extrusion</t>
+  </si>
+  <si>
+    <t>Double pane IGU</t>
+  </si>
+  <si>
+    <t>Triple pane IGU</t>
+  </si>
+  <si>
+    <t>EPDM membrane</t>
+  </si>
+  <si>
+    <t>Polyisocyanurate board</t>
+  </si>
+  <si>
+    <t>wastage</t>
+  </si>
+  <si>
+    <t>6" galvanized steel stud framing</t>
+  </si>
+  <si>
+    <t>Gypsum wall board</t>
+  </si>
+  <si>
+    <t>Normalweight concrete, 4000 psi</t>
+  </si>
+  <si>
+    <t>Normalweight concrete, 6000 psi</t>
+  </si>
+  <si>
+    <t>Normalweight concrete, 5000 psi</t>
+  </si>
+  <si>
+    <t>Steel curtain wall system</t>
+  </si>
+  <si>
+    <t>Aluminum curtain wall system</t>
+  </si>
+  <si>
+    <t>Type N mortar</t>
+  </si>
+  <si>
+    <t>4" Mineral wool insulation</t>
+  </si>
+  <si>
+    <t>4.5" Mineral wool insulation</t>
+  </si>
+  <si>
+    <t>Glass fiber reinforced concrete (GFRC) Panel</t>
+  </si>
+  <si>
+    <t>3/8" Synthetic stucco</t>
+  </si>
+  <si>
+    <t>Galvanized steel backer tray</t>
+  </si>
+  <si>
+    <t>Steel, sheet</t>
+  </si>
+  <si>
+    <t>Thermal break</t>
+  </si>
+  <si>
+    <t>3.5" Mineral wool insulation</t>
+  </si>
+  <si>
+    <t>6" x 1' Tulipwood/Poplar lumber</t>
+  </si>
+  <si>
+    <t>Formed steel sheet</t>
+  </si>
+  <si>
+    <t>Enamel paint</t>
+  </si>
+  <si>
+    <t>Stainless steel fasteners</t>
+  </si>
+  <si>
+    <t>Galvanized steel support</t>
+  </si>
+  <si>
+    <t>5" Mineral wool insulation</t>
+  </si>
+  <si>
+    <t>Galvanized steel support system</t>
+  </si>
+  <si>
+    <t>enhanced wastage</t>
+  </si>
+  <si>
+    <t>Normalweight concrete, 3000 psi</t>
+  </si>
+  <si>
+    <t>Expanded polystyrene (EPS), board</t>
+  </si>
+  <si>
+    <t>Coarse aggregate</t>
+  </si>
+  <si>
+    <t>Composite wood I-joist</t>
+  </si>
+  <si>
+    <t>Oriented strandboard (OSB)</t>
+  </si>
+  <si>
+    <t>Light wood framing</t>
+  </si>
+  <si>
+    <t>Fiberglass blanket insulation, paper faced</t>
+  </si>
+  <si>
+    <t>Window frame, vinyl, fixed</t>
+  </si>
+  <si>
+    <t>SBS modified asphalt shingles</t>
+  </si>
+  <si>
+    <t>Self-adhering, polymer-modified asphalt sheet underlayment</t>
+  </si>
+  <si>
     <t>Steel decking, galvanized</t>
-  </si>
-  <si>
-    <t>Steel, hot rolled structural steel</t>
-  </si>
-  <si>
-    <t>CLT (Cross laminated timber)</t>
-  </si>
-  <si>
-    <t>Glue laminated timber (Glulam)</t>
-  </si>
-  <si>
-    <t>Fluoropolymer coating, metal stock</t>
-  </si>
-  <si>
-    <t>Acrylic latex paint</t>
-  </si>
-  <si>
-    <t>Brick</t>
-  </si>
-  <si>
-    <t>Galvanized steel shelf angle with knife plate</t>
-  </si>
-  <si>
-    <t>AVB membrane</t>
-  </si>
-  <si>
-    <t>Sheathing</t>
-  </si>
-  <si>
-    <t>4" granite veneer</t>
-  </si>
-  <si>
-    <t>Type S mortar</t>
-  </si>
-  <si>
-    <t>Insulated 24 ga. steel sandwich panel with polyurethane foam</t>
-  </si>
-  <si>
-    <t>Fluoropolymer coating</t>
-  </si>
-  <si>
-    <t>Stainless steel fastener</t>
-  </si>
-  <si>
-    <t>2.5" XPS insulation</t>
-  </si>
-  <si>
-    <t>3/4" Brick</t>
-  </si>
-  <si>
-    <t>Water based stain</t>
-  </si>
-  <si>
-    <t>Aluminum extrusion</t>
-  </si>
-  <si>
-    <t>Double pane IGU</t>
-  </si>
-  <si>
-    <t>Triple pane IGU</t>
-  </si>
-  <si>
-    <t>EPDM membrane</t>
-  </si>
-  <si>
-    <t>Polyisocyanurate board</t>
-  </si>
-  <si>
-    <t>wastage</t>
-  </si>
-  <si>
-    <t>6" galvanized steel stud framing</t>
-  </si>
-  <si>
-    <t>Gypsum wall board</t>
-  </si>
-  <si>
-    <t>Normalweight concrete, 4000 psi</t>
-  </si>
-  <si>
-    <t>Normalweight concrete, 6000 psi</t>
-  </si>
-  <si>
-    <t>Normalweight concrete, 5000 psi</t>
-  </si>
-  <si>
-    <t>Steel curtain wall system</t>
-  </si>
-  <si>
-    <t>Aluminum curtain wall system</t>
-  </si>
-  <si>
-    <t>Type N mortar</t>
-  </si>
-  <si>
-    <t>4" Mineral wool insulation</t>
-  </si>
-  <si>
-    <t>4.5" Mineral wool insulation</t>
-  </si>
-  <si>
-    <t>Glass fiber reinforced concrete (GFRC) Panel</t>
-  </si>
-  <si>
-    <t>3/8" Synthetic stucco</t>
-  </si>
-  <si>
-    <t>Galvanized steel backer tray</t>
-  </si>
-  <si>
-    <t>Steel, sheet</t>
-  </si>
-  <si>
-    <t>Thermal break</t>
-  </si>
-  <si>
-    <t>3.5" Mineral wool insulation</t>
-  </si>
-  <si>
-    <t>6" x 1' Tulipwood/Poplar lumber</t>
-  </si>
-  <si>
-    <t>Formed steel sheet</t>
-  </si>
-  <si>
-    <t>Enamel paint</t>
-  </si>
-  <si>
-    <t>Stainless steel fasteners</t>
-  </si>
-  <si>
-    <t>Galvanized steel support</t>
-  </si>
-  <si>
-    <t>5" Mineral wool insulation</t>
-  </si>
-  <si>
-    <t>Galvanized steel support system</t>
-  </si>
-  <si>
-    <t>enhanced wastage</t>
-  </si>
-  <si>
-    <t>Normalweight concrete, 3000 psi</t>
-  </si>
-  <si>
-    <t>Expanded polystyrene (EPS), board</t>
-  </si>
-  <si>
-    <t>Coarse aggregate</t>
-  </si>
-  <si>
-    <t>Composite wood I-joist</t>
-  </si>
-  <si>
-    <t>Oriented strandboard (OSB)</t>
-  </si>
-  <si>
-    <t>Light wood framing</t>
-  </si>
-  <si>
-    <t>Fiberglass blanket insulation, paper faced</t>
-  </si>
-  <si>
-    <t>Window frame, vinyl, fixed</t>
-  </si>
-  <si>
-    <t>SBS modified asphalt shingles</t>
-  </si>
-  <si>
-    <t>Self-adhering, polymer-modified asphalt sheet underlayment</t>
   </si>
 </sst>
 </file>
@@ -570,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53:C53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -584,15 +584,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2">
         <v>0.05</v>
@@ -603,7 +603,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>0.05</v>
@@ -647,7 +647,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="B7">
         <v>0.1</v>
@@ -658,7 +658,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>0.05</v>
@@ -669,7 +669,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9">
         <v>0.05</v>
@@ -680,7 +680,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10">
         <v>0.1</v>
@@ -691,7 +691,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11">
         <v>0.1</v>
@@ -702,7 +702,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12">
         <v>0.1</v>
@@ -713,7 +713,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B13">
         <v>0.05</v>
@@ -724,7 +724,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14">
         <v>0.03</v>
@@ -735,7 +735,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15">
         <v>0.1</v>
@@ -746,7 +746,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16">
         <v>0.03</v>
@@ -757,7 +757,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17">
         <v>0.15</v>
@@ -768,7 +768,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18">
         <v>0.1</v>
@@ -779,7 +779,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19">
         <v>0.01</v>
@@ -790,7 +790,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20">
         <v>0.05</v>
@@ -801,7 +801,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21">
         <v>0.15</v>
@@ -812,7 +812,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22">
         <v>0.1</v>
@@ -823,7 +823,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23">
         <v>0.1</v>
@@ -834,7 +834,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B24">
         <v>0.1</v>
@@ -845,7 +845,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B25">
         <v>0.15</v>
@@ -856,7 +856,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B26">
         <v>0.1</v>
@@ -867,7 +867,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B27">
         <v>0.15</v>
@@ -878,7 +878,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B28">
         <v>0.05</v>
@@ -889,7 +889,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B29">
         <v>0.1</v>
@@ -900,7 +900,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B30">
         <v>0.05</v>
@@ -911,7 +911,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31">
         <v>0.15</v>
@@ -922,7 +922,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B32">
         <v>0.15</v>
@@ -933,7 +933,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B33">
         <v>0.15</v>
@@ -944,7 +944,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B34">
         <v>0.15</v>
@@ -955,7 +955,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B35">
         <v>0.1</v>
@@ -966,7 +966,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36">
         <v>0.1</v>
@@ -977,7 +977,7 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B37">
         <v>0.05</v>
@@ -988,7 +988,7 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B38">
         <v>0.1</v>
@@ -999,7 +999,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B39">
         <v>0.1</v>
@@ -1010,7 +1010,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B40">
         <v>0.05</v>
@@ -1021,7 +1021,7 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41">
         <v>0.1</v>
@@ -1032,7 +1032,7 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B42">
         <v>0.1</v>
@@ -1043,7 +1043,7 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B43">
         <v>0.1</v>
@@ -1054,7 +1054,7 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B44">
         <v>0.1</v>
@@ -1065,7 +1065,7 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45">
         <v>0.1</v>
@@ -1076,7 +1076,7 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46">
         <v>0.1</v>
@@ -1087,7 +1087,7 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B47">
         <v>0.05</v>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48">
         <v>0.1</v>
@@ -1109,7 +1109,7 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B49">
         <v>0.01</v>
@@ -1120,7 +1120,7 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B50">
         <v>0.01</v>
@@ -1131,7 +1131,7 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B51">
         <v>0.15</v>
@@ -1142,7 +1142,7 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B52">
         <v>0.15</v>
@@ -1153,7 +1153,7 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B53">
         <v>0.15</v>
@@ -1164,7 +1164,7 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B54">
         <v>0.1</v>
@@ -1175,7 +1175,7 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B55">
         <v>0.1</v>
@@ -1186,7 +1186,7 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B56">
         <v>0.1</v>
@@ -1197,7 +1197,7 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B57">
         <v>0.1</v>
@@ -1208,7 +1208,7 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B58">
         <v>0.1</v>
@@ -1219,7 +1219,7 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B59">
         <v>0.1</v>
@@ -1230,7 +1230,7 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B60">
         <v>0.1</v>

</xml_diff>